<commit_message>
EPBDS-8851 add a tooltip and a link in Webstudio if Datatype is created via constructor, fix cast factory from Alias to Type and vise versa, added ability to validate a message of domain validation exception in Test tables if it happens in runtime
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7847_Cast_Object_To_Alias.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7847_Cast_Object_To_Alias.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86280ED3-F533-4F0C-8881-5BD77471E002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Datatype MyDataType</t>
   </si>
@@ -92,11 +93,35 @@
   <si>
     <t>= new HashMap().get("DT");</t>
   </si>
+  <si>
+    <t>Datatype Gender &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult test2()</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>M:Gender</t>
+  </si>
+  <si>
+    <t>= $OBJ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -157,10 +182,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -168,14 +198,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,9 +246,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,9 +281,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,9 +333,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,26 +525,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -485,7 +552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -493,7 +560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -501,7 +568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -509,21 +576,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -531,7 +598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -539,7 +606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
@@ -547,7 +614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
@@ -555,7 +622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
@@ -563,7 +630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -571,7 +638,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="79.8" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -579,28 +646,79 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1"/>
     </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>